<commit_message>
Emily update week7 timesheet
</commit_message>
<xml_diff>
--- a/Agenda_Minutes_Timesheet/Time sheet/Timetsheet - Yingyao Lu.xlsx
+++ b/Agenda_Minutes_Timesheet/Time sheet/Timetsheet - Yingyao Lu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emily/Desktop/mindspace/Time sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emily/Desktop/mindspace/Agenda_Minutes_Timesheet/Time sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889A40C2-1D13-0449-A1B6-2397662A0A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26209934-4304-FB44-926B-7732F6095F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="500" windowWidth="24540" windowHeight="17500" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="500" windowWidth="24540" windowHeight="17500" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week2" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Week5" sheetId="1" r:id="rId4"/>
     <sheet name="Week6" sheetId="5" r:id="rId5"/>
     <sheet name="Midbreak" sheetId="6" r:id="rId6"/>
+    <sheet name="Week7" sheetId="8" r:id="rId7"/>
+    <sheet name="Week8" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Midbreak!$A$1:$H$21</definedName>
@@ -27,11 +29,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">Week4!$A$1:$H$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Week5!$A$1:$H$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">Week6!$A$1:$H$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Week7!$A$1:$H$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">Week8!$A$1:$H$14</definedName>
     <definedName name="Week_Start" localSheetId="5">Midbreak!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="0">Week2!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="1">Week3!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="2">Week4!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="4">Week6!$C$4</definedName>
+    <definedName name="Week_Start" localSheetId="6">Week7!$C$4</definedName>
+    <definedName name="Week_Start" localSheetId="7">Week8!$C$4</definedName>
     <definedName name="Week_Start">Week5!$C$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -53,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="132">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -418,6 +424,45 @@
   </si>
   <si>
     <t>Working on Dashboard with user data</t>
+  </si>
+  <si>
+    <t>Work on insights page</t>
+  </si>
+  <si>
+    <t>Work on insight front end basic look</t>
+  </si>
+  <si>
+    <t>Work on fetching data with backend</t>
+  </si>
+  <si>
+    <t>Client Meeting + Team Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present mailstone 1 development </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For fetching data from backend </t>
+  </si>
+  <si>
+    <t>Work on milestone 1 report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepare mileston 1 report </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan, organise and track project development process </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write milestone 1 report </t>
+  </si>
+  <si>
+    <t>Work on Subscribtion</t>
+  </si>
+  <si>
+    <t>Fix bugs</t>
+  </si>
+  <si>
+    <t>Finish insights hashtag function</t>
   </si>
 </sst>
 </file>
@@ -625,11 +670,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -992,16 +1037,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1622,16 +1667,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2383,16 +2428,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3208,16 +3253,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3926,16 +3971,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -4495,8 +4540,8 @@
   </sheetPr>
   <dimension ref="A2:AW20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4512,16 +4557,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -4539,7 +4584,7 @@
       <c r="G3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="23" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4580,7 +4625,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="15">
-        <v>44299</v>
+        <v>44298</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
@@ -4635,7 +4680,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="15">
-        <v>44300</v>
+        <v>44299</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -4690,7 +4735,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="15">
-        <v>44301</v>
+        <v>44300</v>
       </c>
       <c r="C8" s="16">
         <v>0.58333333333333337</v>
@@ -4757,7 +4802,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="15">
-        <v>44302</v>
+        <v>44301</v>
       </c>
       <c r="C9" s="16">
         <v>0.625</v>
@@ -4824,7 +4869,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="15">
-        <v>44303</v>
+        <v>44302</v>
       </c>
       <c r="C10" s="16">
         <v>0.66666666666666663</v>
@@ -4891,7 +4936,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="15">
-        <v>44304</v>
+        <v>44303</v>
       </c>
       <c r="C11" s="16">
         <v>0.58333333333333337</v>
@@ -4958,7 +5003,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="15">
-        <v>44305</v>
+        <v>44304</v>
       </c>
       <c r="C12" s="16">
         <v>0.58333333333333337</v>
@@ -5025,7 +5070,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="15">
-        <v>44306</v>
+        <v>44305</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -5080,7 +5125,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="15">
-        <v>44307</v>
+        <v>44306</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
@@ -5135,7 +5180,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="15">
-        <v>44308</v>
+        <v>44307</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -5190,7 +5235,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="15">
-        <v>44309</v>
+        <v>44308</v>
       </c>
       <c r="C16" s="16">
         <v>0.58333333333333337</v>
@@ -5255,7 +5300,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="15">
-        <v>44310</v>
+        <v>44309</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -5310,7 +5355,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="15">
-        <v>44311</v>
+        <v>44310</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -5365,7 +5410,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="15">
-        <v>44312</v>
+        <v>44311</v>
       </c>
       <c r="C19" s="16">
         <v>0.66666666666666663</v>
@@ -5455,4 +5500,1145 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5F1514-9985-D049-931F-0495C4EC828D}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:AW14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="15" max="49" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1784870</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="15">
+        <v>44312</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E6" s="13">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
+      <c r="AK6" s="9"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="9"/>
+    </row>
+    <row r="7" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="15">
+        <v>44313</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="13">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="9"/>
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="9"/>
+      <c r="AW7" s="9"/>
+    </row>
+    <row r="8" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0.875</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="9"/>
+      <c r="AS8" s="9"/>
+      <c r="AT8" s="9"/>
+      <c r="AU8" s="9"/>
+      <c r="AV8" s="9"/>
+      <c r="AW8" s="9"/>
+    </row>
+    <row r="9" spans="1:49" s="10" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="15">
+        <v>44314</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E9" s="13">
+        <v>4</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="9"/>
+      <c r="AT9" s="9"/>
+      <c r="AU9" s="9"/>
+      <c r="AV9" s="9"/>
+      <c r="AW9" s="9"/>
+    </row>
+    <row r="10" spans="1:49" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="15">
+        <v>44315</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="E10" s="13">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="9"/>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="9"/>
+      <c r="AT10" s="9"/>
+      <c r="AU10" s="9"/>
+      <c r="AV10" s="9"/>
+      <c r="AW10" s="9"/>
+    </row>
+    <row r="11" spans="1:49" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="15">
+        <v>44316</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E11" s="13">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
+      <c r="AT11" s="9"/>
+      <c r="AU11" s="9"/>
+      <c r="AV11" s="9"/>
+      <c r="AW11" s="9"/>
+    </row>
+    <row r="12" spans="1:49" s="10" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="15">
+        <v>44317</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E12" s="13">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="9"/>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="9"/>
+      <c r="AT12" s="9"/>
+      <c r="AU12" s="9"/>
+      <c r="AV12" s="9"/>
+      <c r="AW12" s="9"/>
+    </row>
+    <row r="13" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="15">
+        <v>44318</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E13" s="13">
+        <v>4</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+      <c r="AK13" s="9"/>
+      <c r="AL13" s="9"/>
+      <c r="AM13" s="9"/>
+      <c r="AN13" s="9"/>
+      <c r="AO13" s="9"/>
+      <c r="AP13" s="9"/>
+      <c r="AQ13" s="9"/>
+      <c r="AR13" s="9"/>
+      <c r="AS13" s="9"/>
+      <c r="AT13" s="9"/>
+      <c r="AU13" s="9"/>
+      <c r="AV13" s="9"/>
+      <c r="AW13" s="9"/>
+    </row>
+    <row r="14" spans="1:49" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="8">
+        <f>SUM(E6:E13)</f>
+        <v>22</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D13" xr:uid="{B3EAE523-0C40-B54A-9350-8B1AFBED8DE4}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4699F877-352F-5F4D-B12B-C810CDF9746F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:AW13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="15" max="49" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1784870</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="15">
+        <v>44319</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
+      <c r="AK6" s="9"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="9"/>
+    </row>
+    <row r="7" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="15">
+        <v>44320</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="9"/>
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="9"/>
+      <c r="AW7" s="9"/>
+    </row>
+    <row r="8" spans="1:49" s="10" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="15">
+        <v>44321</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="9"/>
+      <c r="AS8" s="9"/>
+      <c r="AT8" s="9"/>
+      <c r="AU8" s="9"/>
+      <c r="AV8" s="9"/>
+      <c r="AW8" s="9"/>
+    </row>
+    <row r="9" spans="1:49" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="15">
+        <v>44322</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="9"/>
+      <c r="AT9" s="9"/>
+      <c r="AU9" s="9"/>
+      <c r="AV9" s="9"/>
+      <c r="AW9" s="9"/>
+    </row>
+    <row r="10" spans="1:49" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="15">
+        <v>44323</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="9"/>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="9"/>
+      <c r="AT10" s="9"/>
+      <c r="AU10" s="9"/>
+      <c r="AV10" s="9"/>
+      <c r="AW10" s="9"/>
+    </row>
+    <row r="11" spans="1:49" s="10" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="15">
+        <v>44324</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
+      <c r="AT11" s="9"/>
+      <c r="AU11" s="9"/>
+      <c r="AV11" s="9"/>
+      <c r="AW11" s="9"/>
+    </row>
+    <row r="12" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="15">
+        <v>44325</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="9"/>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="9"/>
+      <c r="AT12" s="9"/>
+      <c r="AU12" s="9"/>
+      <c r="AV12" s="9"/>
+      <c r="AW12" s="9"/>
+    </row>
+    <row r="13" spans="1:49" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="8">
+        <f>SUM(E6:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D12" xr:uid="{987EAD20-1428-8B49-9AA3-4B6D14478A7A}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Emily updated week 8 timesheet
</commit_message>
<xml_diff>
--- a/Agenda_Minutes_Timesheet/Time sheet/Timetsheet - Yingyao Lu.xlsx
+++ b/Agenda_Minutes_Timesheet/Time sheet/Timetsheet - Yingyao Lu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emily/Desktop/mindspace/Agenda_Minutes_Timesheet/Time sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emily/Desktop/Team-024/Agenda_Minutes_Timesheet/Time sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26209934-4304-FB44-926B-7732F6095F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63266B07-DAC3-0747-974A-2B55D5BCF97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="500" windowWidth="24540" windowHeight="17500" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <sheet name="Midbreak" sheetId="6" r:id="rId6"/>
     <sheet name="Week7" sheetId="8" r:id="rId7"/>
     <sheet name="Week8" sheetId="9" r:id="rId8"/>
+    <sheet name="Week9" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Midbreak!$A$1:$H$21</definedName>
@@ -31,6 +32,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="4">Week6!$A$1:$H$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">Week7!$A$1:$H$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">Week8!$A$1:$H$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">Week9!$A$1:$H$14</definedName>
     <definedName name="Week_Start" localSheetId="5">Midbreak!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="0">Week2!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="1">Week3!$C$4</definedName>
@@ -38,6 +40,7 @@
     <definedName name="Week_Start" localSheetId="4">Week6!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="6">Week7!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="7">Week8!$C$4</definedName>
+    <definedName name="Week_Start" localSheetId="8">Week9!$C$4</definedName>
     <definedName name="Week_Start">Week5!$C$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -59,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="142">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -463,6 +466,36 @@
   </si>
   <si>
     <t>Finish insights hashtag function</t>
+  </si>
+  <si>
+    <t>Final Milestone plan</t>
+  </si>
+  <si>
+    <t>Plan for milestone 2</t>
+  </si>
+  <si>
+    <t>Develop Timeline page</t>
+  </si>
+  <si>
+    <t>Develop Hashtag function</t>
+  </si>
+  <si>
+    <t>Develop Modal page</t>
+  </si>
+  <si>
+    <t>milestone 2 task</t>
+  </si>
+  <si>
+    <t>Frontend in progress 90%</t>
+  </si>
+  <si>
+    <t>Frontend in progress 50%</t>
+  </si>
+  <si>
+    <t>Finish front end part description draft</t>
+  </si>
+  <si>
+    <t>Frontend finished 60%</t>
   </si>
 </sst>
 </file>
@@ -5510,7 +5543,7 @@
   <dimension ref="A2:AW14"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C7" sqref="C7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6149,7 +6182,7 @@
   <dimension ref="A2:AW13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:H12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6234,6 +6267,580 @@
       </c>
       <c r="B6" s="15">
         <v>44319</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="E6" s="13">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
+      <c r="AK6" s="9"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="9"/>
+    </row>
+    <row r="7" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="15">
+        <v>44320</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.875</v>
+      </c>
+      <c r="E7" s="13">
+        <v>8</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="9"/>
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="9"/>
+      <c r="AW7" s="9"/>
+    </row>
+    <row r="8" spans="1:49" s="10" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="15">
+        <v>44321</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="9"/>
+      <c r="AS8" s="9"/>
+      <c r="AT8" s="9"/>
+      <c r="AU8" s="9"/>
+      <c r="AV8" s="9"/>
+      <c r="AW8" s="9"/>
+    </row>
+    <row r="9" spans="1:49" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="15">
+        <v>44322</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E9" s="13">
+        <v>6</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="9"/>
+      <c r="AT9" s="9"/>
+      <c r="AU9" s="9"/>
+      <c r="AV9" s="9"/>
+      <c r="AW9" s="9"/>
+    </row>
+    <row r="10" spans="1:49" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="15">
+        <v>44323</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E10" s="13">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="9"/>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="9"/>
+      <c r="AT10" s="9"/>
+      <c r="AU10" s="9"/>
+      <c r="AV10" s="9"/>
+      <c r="AW10" s="9"/>
+    </row>
+    <row r="11" spans="1:49" s="10" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="15">
+        <v>44324</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E11" s="13">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
+      <c r="AT11" s="9"/>
+      <c r="AU11" s="9"/>
+      <c r="AV11" s="9"/>
+      <c r="AW11" s="9"/>
+    </row>
+    <row r="12" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="15">
+        <v>44325</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="9"/>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="9"/>
+      <c r="AT12" s="9"/>
+      <c r="AU12" s="9"/>
+      <c r="AV12" s="9"/>
+      <c r="AW12" s="9"/>
+    </row>
+    <row r="13" spans="1:49" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="8">
+        <f>SUM(E6:E12)</f>
+        <v>24</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D12" xr:uid="{987EAD20-1428-8B49-9AA3-4B6D14478A7A}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EDBA09D-23BF-4445-9D7A-E9193B36B168}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:AW13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="15" max="49" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1784870</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="15">
+        <v>44326</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
@@ -6288,7 +6895,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="15">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -6343,7 +6950,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="15">
-        <v>44321</v>
+        <v>44328</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
@@ -6398,7 +7005,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="15">
-        <v>44322</v>
+        <v>44329</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -6453,7 +7060,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="15">
-        <v>44323</v>
+        <v>44330</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -6508,7 +7115,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="15">
-        <v>44324</v>
+        <v>44331</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -6563,7 +7170,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="15">
-        <v>44325</v>
+        <v>44332</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -6633,7 +7240,7 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D12" xr:uid="{987EAD20-1428-8B49-9AA3-4B6D14478A7A}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D12" xr:uid="{B8B5D74A-DB8A-9245-9027-D1625EDF6807}">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Update Timetsheet - Yingyao Lu.xlsx
</commit_message>
<xml_diff>
--- a/Agenda_Minutes_Timesheet/Time sheet/Timetsheet - Yingyao Lu.xlsx
+++ b/Agenda_Minutes_Timesheet/Time sheet/Timetsheet - Yingyao Lu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emily/Desktop/Team-024/Agenda_Minutes_Timesheet/Time sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63266B07-DAC3-0747-974A-2B55D5BCF97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E46088-F711-884E-BD73-4F931174C370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="500" windowWidth="24540" windowHeight="17500" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="500" windowWidth="24540" windowHeight="17500" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week2" sheetId="3" r:id="rId1"/>
@@ -22,9 +22,13 @@
     <sheet name="Week7" sheetId="8" r:id="rId7"/>
     <sheet name="Week8" sheetId="9" r:id="rId8"/>
     <sheet name="Week9" sheetId="10" r:id="rId9"/>
+    <sheet name="Week10" sheetId="11" r:id="rId10"/>
+    <sheet name="Week11" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Midbreak!$A$1:$H$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">Week10!$A$1:$H$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">Week11!$A$1:$H$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Week2!$A$1:$H$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Week3!$A$1:$H$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Week4!$A$1:$H$18</definedName>
@@ -34,6 +38,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="7">Week8!$A$1:$H$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">Week9!$A$1:$H$14</definedName>
     <definedName name="Week_Start" localSheetId="5">Midbreak!$C$4</definedName>
+    <definedName name="Week_Start" localSheetId="9">Week10!$C$4</definedName>
+    <definedName name="Week_Start" localSheetId="10">Week11!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="0">Week2!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="1">Week3!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="2">Week4!$C$4</definedName>
@@ -62,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="153">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -496,6 +502,39 @@
   </si>
   <si>
     <t>Frontend finished 60%</t>
+  </si>
+  <si>
+    <t>Testing Plan</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client meeting </t>
+  </si>
+  <si>
+    <t>Prepare Client Meeting</t>
+  </si>
+  <si>
+    <t>Cllient meeting</t>
+  </si>
+  <si>
+    <t>First draft</t>
+  </si>
+  <si>
+    <t>Work on database</t>
+  </si>
+  <si>
+    <t>Defects tesing</t>
+  </si>
+  <si>
+    <t>Integration testing</t>
+  </si>
+  <si>
+    <t>Prepare for client meeting and testing</t>
+  </si>
+  <si>
+    <t>Work on timeline layout</t>
   </si>
 </sst>
 </file>
@@ -1677,6 +1716,1098 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AE3FFC-E12A-8844-A17A-C55F5E9E3F50}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:AW13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="15" max="49" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1784870</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="15">
+        <v>44333</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="E6" s="13">
+        <v>4</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
+      <c r="AK6" s="9"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="9"/>
+    </row>
+    <row r="7" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="15">
+        <v>44334</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.875</v>
+      </c>
+      <c r="E7" s="13">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="9"/>
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="9"/>
+      <c r="AW7" s="9"/>
+    </row>
+    <row r="8" spans="1:49" s="10" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="15">
+        <v>44335</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0</v>
+      </c>
+      <c r="E8" s="13">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="9"/>
+      <c r="AS8" s="9"/>
+      <c r="AT8" s="9"/>
+      <c r="AU8" s="9"/>
+      <c r="AV8" s="9"/>
+      <c r="AW8" s="9"/>
+    </row>
+    <row r="9" spans="1:49" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="15">
+        <v>44336</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E9" s="13">
+        <v>6</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="9"/>
+      <c r="AT9" s="9"/>
+      <c r="AU9" s="9"/>
+      <c r="AV9" s="9"/>
+      <c r="AW9" s="9"/>
+    </row>
+    <row r="10" spans="1:49" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="15">
+        <v>44337</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.875</v>
+      </c>
+      <c r="E10" s="13">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="9"/>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="9"/>
+      <c r="AT10" s="9"/>
+      <c r="AU10" s="9"/>
+      <c r="AV10" s="9"/>
+      <c r="AW10" s="9"/>
+    </row>
+    <row r="11" spans="1:49" s="10" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="15">
+        <v>44338</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="E11" s="13">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
+      <c r="AT11" s="9"/>
+      <c r="AU11" s="9"/>
+      <c r="AV11" s="9"/>
+      <c r="AW11" s="9"/>
+    </row>
+    <row r="12" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="15">
+        <v>44339</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="9"/>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="9"/>
+      <c r="AT12" s="9"/>
+      <c r="AU12" s="9"/>
+      <c r="AV12" s="9"/>
+      <c r="AW12" s="9"/>
+    </row>
+    <row r="13" spans="1:49" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="8">
+        <f>SUM(E6:E12)</f>
+        <v>21</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D12" xr:uid="{26BB8373-2390-EB41-B124-F9877B931D63}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E21D489-BB62-4E4F-B505-4DA86C21F6F7}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:AW13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="15" max="49" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1784870</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="15">
+        <v>44340</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="13">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
+      <c r="AK6" s="9"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="9"/>
+    </row>
+    <row r="7" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="15">
+        <v>44341</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="9"/>
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="9"/>
+      <c r="AW7" s="9"/>
+    </row>
+    <row r="8" spans="1:49" s="10" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="15">
+        <v>44342</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="9"/>
+      <c r="AS8" s="9"/>
+      <c r="AT8" s="9"/>
+      <c r="AU8" s="9"/>
+      <c r="AV8" s="9"/>
+      <c r="AW8" s="9"/>
+    </row>
+    <row r="9" spans="1:49" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="15">
+        <v>44343</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="9"/>
+      <c r="AT9" s="9"/>
+      <c r="AU9" s="9"/>
+      <c r="AV9" s="9"/>
+      <c r="AW9" s="9"/>
+    </row>
+    <row r="10" spans="1:49" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="15">
+        <v>44344</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="9"/>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="9"/>
+      <c r="AT10" s="9"/>
+      <c r="AU10" s="9"/>
+      <c r="AV10" s="9"/>
+      <c r="AW10" s="9"/>
+    </row>
+    <row r="11" spans="1:49" s="10" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="15">
+        <v>44345</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
+      <c r="AT11" s="9"/>
+      <c r="AU11" s="9"/>
+      <c r="AV11" s="9"/>
+      <c r="AW11" s="9"/>
+    </row>
+    <row r="12" spans="1:49" s="10" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="15">
+        <v>44346</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="9"/>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="9"/>
+      <c r="AT12" s="9"/>
+      <c r="AU12" s="9"/>
+      <c r="AV12" s="9"/>
+      <c r="AW12" s="9"/>
+    </row>
+    <row r="13" spans="1:49" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="8">
+        <f>SUM(E6:E12)</f>
+        <v>2</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D12" xr:uid="{1E4BCC00-D266-7E4C-BCFC-EED12C7739F7}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8638C716-9BEC-5048-BA69-2BE325348D01}">
   <sheetPr>
@@ -5543,7 +6674,7 @@
   <dimension ref="A2:AW14"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5587,7 +6718,7 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
@@ -6181,8 +7312,8 @@
   </sheetPr>
   <dimension ref="A2:AW13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6226,7 +7357,7 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
@@ -6756,7 +7887,7 @@
   <dimension ref="A2:AW13"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6800,7 +7931,7 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
@@ -6842,11 +7973,21 @@
       <c r="B6" s="15">
         <v>44326</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="C6" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="E6" s="13">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>137</v>
+      </c>
       <c r="H6" s="11"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -6897,11 +8038,21 @@
       <c r="B7" s="15">
         <v>44327</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="C7" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.875</v>
+      </c>
+      <c r="E7" s="13">
+        <v>7</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>137</v>
+      </c>
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -6952,12 +8103,24 @@
       <c r="B8" s="15">
         <v>44328</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="11"/>
+      <c r="C8" s="16">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>149</v>
+      </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -7007,12 +8170,24 @@
       <c r="B9" s="15">
         <v>44329</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="11"/>
+      <c r="C9" s="16">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E9" s="13">
+        <v>2</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>150</v>
+      </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -7062,11 +8237,21 @@
       <c r="B10" s="15">
         <v>44330</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="C10" s="16">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E10" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>151</v>
+      </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -7117,12 +8302,24 @@
       <c r="B11" s="15">
         <v>44331</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="11"/>
+      <c r="C11" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E11" s="13">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>147</v>
+      </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -7226,7 +8423,7 @@
       </c>
       <c r="E13" s="8">
         <f>SUM(E6:E12)</f>
-        <v>0</v>
+        <v>20.5</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>

</xml_diff>